<commit_message>
course status fields-courses images academic staff remove filtering
</commit_message>
<xml_diff>
--- a/public/Excel/academic_staff.xlsx
+++ b/public/Excel/academic_staff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ziead\Desktop\laravel projects\portfolio\public\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5238E531-8373-4C9D-9A59-D1ACE39706AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1968E528-6297-4355-962F-43675401AD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,8 +259,8 @@
     <tableColumn id="4" xr3:uid="{2A4DD1BA-C045-495E-AC51-35D023C46B0D}" name="phone_number" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{8A58FFCA-E84D-4832-AC78-AFFC6DC73DE8}" name="img" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{F63F25F7-6726-4B25-A137-DD0C01B5B572}" name="department" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{84E07D60-6036-45AE-86BA-7C1C7E85F2DE}" name="title" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{6BE36A6E-4456-43C7-B193-990608D4EBC1}" name="degree" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{84E07D60-6036-45AE-86BA-7C1C7E85F2DE}" name="title" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{6BE36A6E-4456-43C7-B193-990608D4EBC1}" name="degree" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -532,7 +532,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
excel and upload updates
</commit_message>
<xml_diff>
--- a/public/Excel/academic_staff.xlsx
+++ b/public/Excel/academic_staff.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ziead\Desktop\laravel projects\portfolio\public\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1968E528-6297-4355-962F-43675401AD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B431D8-1CB9-4022-9E61-85FBFD8160E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2412" yWindow="1488" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="96">
   <si>
     <t>name</t>
   </si>
@@ -66,54 +66,6 @@
     <t>images/Dr.Ahmed-Younes.png</t>
   </si>
   <si>
-    <t>waled@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waled </t>
-  </si>
-  <si>
-    <t>magdy</t>
-  </si>
-  <si>
-    <t>magdy@gmail.com</t>
-  </si>
-  <si>
-    <t>mohamed</t>
-  </si>
-  <si>
-    <t>mohamed@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ahmed </t>
-  </si>
-  <si>
-    <t>youne@gmail.com</t>
-  </si>
-  <si>
-    <t>youn@gmail.com</t>
-  </si>
-  <si>
-    <t>you@gmail.com</t>
-  </si>
-  <si>
-    <t>yo@gmail.com</t>
-  </si>
-  <si>
-    <t>y@gmail.com</t>
-  </si>
-  <si>
-    <t>fghjhg@gmail.com</t>
-  </si>
-  <si>
-    <t>ghjkklhj@gmail.com</t>
-  </si>
-  <si>
-    <t>dhjghgfk@gmail.com</t>
-  </si>
-  <si>
-    <t>ghjfjfgjkfgj@gmail.com</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -121,6 +73,246 @@
   </si>
   <si>
     <t>instructor</t>
+  </si>
+  <si>
+    <t>Rasha Montaser</t>
+  </si>
+  <si>
+    <t>Shimaa Elmorsy</t>
+  </si>
+  <si>
+    <t>Islam Elkabani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohamed El Kholy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geihan Al Ashry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emad Raouf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amira El Sayed </t>
+  </si>
+  <si>
+    <t>El Sayed Mostafa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohamed Saad </t>
+  </si>
+  <si>
+    <t>Hala Idriss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nermin Kashef </t>
+  </si>
+  <si>
+    <t>Marwa Abdel Hamid</t>
+  </si>
+  <si>
+    <t>Mai Ahmed</t>
+  </si>
+  <si>
+    <t>Mahmoud Matrawy</t>
+  </si>
+  <si>
+    <t>Noura Nasr</t>
+  </si>
+  <si>
+    <t>Youstina Nabil</t>
+  </si>
+  <si>
+    <t>Sara Anwer</t>
+  </si>
+  <si>
+    <t>Ahmed Saleh</t>
+  </si>
+  <si>
+    <t>Ahmed Ramadan</t>
+  </si>
+  <si>
+    <t>Mirna Hosny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmed Mostafa </t>
+  </si>
+  <si>
+    <t>enna El Masry</t>
+  </si>
+  <si>
+    <t>01270599963</t>
+  </si>
+  <si>
+    <t>01006020406</t>
+  </si>
+  <si>
+    <t>01004848151</t>
+  </si>
+  <si>
+    <t>01220144633</t>
+  </si>
+  <si>
+    <t>01111738681</t>
+  </si>
+  <si>
+    <t>01224281043</t>
+  </si>
+  <si>
+    <t>01203238502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hatem Abdalkader </t>
+  </si>
+  <si>
+    <t>01003701988</t>
+  </si>
+  <si>
+    <t>01285921970</t>
+  </si>
+  <si>
+    <t>01110003193</t>
+  </si>
+  <si>
+    <t>01000483840</t>
+  </si>
+  <si>
+    <t>01005017369</t>
+  </si>
+  <si>
+    <t>01011524271</t>
+  </si>
+  <si>
+    <t>01124343824</t>
+  </si>
+  <si>
+    <t>Shimaa@gmail.com</t>
+  </si>
+  <si>
+    <t>Rasha@gmail.com</t>
+  </si>
+  <si>
+    <t>islam@gmail.com</t>
+  </si>
+  <si>
+    <t>MohamedElkholy@gmail.com</t>
+  </si>
+  <si>
+    <t>Geihan@gmail.com</t>
+  </si>
+  <si>
+    <t>Emad@gmail.com</t>
+  </si>
+  <si>
+    <t>Hatem@gmail.com</t>
+  </si>
+  <si>
+    <t>Amira@gmail.com</t>
+  </si>
+  <si>
+    <t>ElSayedmostafa@gmail.com</t>
+  </si>
+  <si>
+    <t>Mohamedsaad@gmail.com</t>
+  </si>
+  <si>
+    <t>Halaidriss@gmail.com</t>
+  </si>
+  <si>
+    <t>Nerminkashef@gmail.com</t>
+  </si>
+  <si>
+    <t>MarwaAbdelhamid@gmail.com</t>
+  </si>
+  <si>
+    <t>Maiahmed@gmail.com</t>
+  </si>
+  <si>
+    <t>Matrawy@gmail.com</t>
+  </si>
+  <si>
+    <t>Nouranasr@gmail.com</t>
+  </si>
+  <si>
+    <t>Youstina@gmail.com</t>
+  </si>
+  <si>
+    <t>Saraanwer@gmail.com</t>
+  </si>
+  <si>
+    <t>AhmedSaleh@gmail.com</t>
+  </si>
+  <si>
+    <t>Ahmedramadan@gmail.com</t>
+  </si>
+  <si>
+    <t>Mirnahosny@gmail.com</t>
+  </si>
+  <si>
+    <t>Ahmedmostafa@gmail.com</t>
+  </si>
+  <si>
+    <t>MennaElmasry@gmail.com</t>
+  </si>
+  <si>
+    <t>01221334341</t>
+  </si>
+  <si>
+    <t>01001233211</t>
+  </si>
+  <si>
+    <t>01289892211</t>
+  </si>
+  <si>
+    <t>01123131231</t>
+  </si>
+  <si>
+    <t>01212903412</t>
+  </si>
+  <si>
+    <t>01189236734</t>
+  </si>
+  <si>
+    <t>01178349801</t>
+  </si>
+  <si>
+    <t>01278365222</t>
+  </si>
+  <si>
+    <t>01278452390</t>
+  </si>
+  <si>
+    <t>01123783252</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1eITcH_AYxa9TXXnXHoYErIz-cfgDfdIt/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1mk-gYAXXP_A9mAXnRjulzaWnmSn5lE0G/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1faq2dBFSVXniNoTvCqgwfLpPMGWJE2mR/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1mIPAQiKufQDIOWZnG1ho8X9wGqXY_xUt/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ahE9fMCNzUYN3_265tK0AQFKvASki0rf/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1nPySm8gA9zM0cdFNho2DszpJIIvjNZqI/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ut8tK4SjTWeY4fNLpwMwhok6P8NhHvuG/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1zwSZkrINxj5nnxuoqw4whNeF5tdnwjUm/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/15gR9_rGPZkEFH_O6b5nIxjvZ0rEljYBA/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/14xU7QRkl8gmXAZ8wJzQHX07VA8YcHeUP/view?usp=drive_link</t>
   </si>
 </sst>
 </file>
@@ -247,20 +439,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3D97EDF-310B-47E9-8004-21214F21EDB8}" name="Table2" displayName="Table2" ref="A1:H14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H14" xr:uid="{C3D97EDF-310B-47E9-8004-21214F21EDB8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:H25" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H25" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H14">
     <sortCondition ref="H1:H14"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{092506A5-E2EC-431D-9201-C671598AA876}" name="name" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{4D650C89-4908-484F-B268-97EEF223B85F}" name="verbose_title" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{582DFB1D-955B-4645-8CE6-AD1198DEC1BA}" name="email" dataDxfId="5" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{2A4DD1BA-C045-495E-AC51-35D023C46B0D}" name="phone_number" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{8A58FFCA-E84D-4832-AC78-AFFC6DC73DE8}" name="img" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{F63F25F7-6726-4B25-A137-DD0C01B5B572}" name="department" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{84E07D60-6036-45AE-86BA-7C1C7E85F2DE}" name="title" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{6BE36A6E-4456-43C7-B193-990608D4EBC1}" name="degree" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="name" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="verbose_title" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="email" dataDxfId="5" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="phone_number" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="img" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="department" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="title" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="degree" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -529,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +758,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -583,17 +775,17 @@
       <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5">
-        <v>8974985</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
+      <c r="D2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>11</v>
@@ -602,16 +794,16 @@
     </row>
     <row r="3" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5">
-        <v>8974986</v>
+        <v>53</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -620,7 +812,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>11</v>
@@ -629,16 +821,16 @@
     </row>
     <row r="4" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="5">
-        <v>8974987</v>
+        <v>54</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>12</v>
@@ -647,7 +839,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>11</v>
@@ -656,25 +848,25 @@
     </row>
     <row r="5" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5">
-        <v>8974988</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>55</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>11</v>
@@ -689,19 +881,19 @@
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="5">
-        <v>8974989</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>56</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>11</v>
@@ -710,15 +902,17 @@
     </row>
     <row r="7" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
@@ -726,7 +920,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>11</v>
@@ -735,16 +929,16 @@
     </row>
     <row r="8" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="5">
-        <v>8974991</v>
+        <v>58</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>12</v>
@@ -753,7 +947,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>11</v>
@@ -762,16 +956,16 @@
     </row>
     <row r="9" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="5">
-        <v>8974992</v>
+        <v>59</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>12</v>
@@ -780,7 +974,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>11</v>
@@ -789,16 +983,16 @@
     </row>
     <row r="10" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="5">
-        <v>8974993</v>
+        <v>60</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>12</v>
@@ -807,7 +1001,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>11</v>
@@ -816,16 +1010,16 @@
     </row>
     <row r="11" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="5">
-        <v>8974994</v>
+        <v>61</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>12</v>
@@ -834,7 +1028,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>11</v>
@@ -843,25 +1037,25 @@
     </row>
     <row r="12" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="5">
-        <v>8974995</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>12</v>
+        <v>62</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>11</v>
@@ -870,25 +1064,25 @@
     </row>
     <row r="13" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="5">
-        <v>8974996</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>12</v>
+        <v>63</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>11</v>
@@ -897,15 +1091,17 @@
     </row>
     <row r="14" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>64</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="E14" s="3" t="s">
         <v>12</v>
       </c>
@@ -913,33 +1109,328 @@
         <v>10</v>
       </c>
       <c r="G14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="1"/>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A4206E37-043C-4637-8C6B-1FC6E8BE8C8D}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{370159B8-5FC6-4F12-A6C1-794A9DEF765E}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{4A2DB56B-74B3-4846-92E8-7420F5C4DB58}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{CA0074BD-8E0B-429D-ACA3-26679EEBBB81}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{1D28AED2-5C59-4210-B437-609F5ABFC1F1}"/>
-    <hyperlink ref="C10" r:id="rId6" xr:uid="{C94FB345-0851-426A-ACC4-7CDF0505F78D}"/>
-    <hyperlink ref="C12" r:id="rId7" xr:uid="{4FCABE8A-303D-4F6C-935B-F0F3C7A32898}"/>
-    <hyperlink ref="C14" r:id="rId8" xr:uid="{1CC84FB6-04A2-4A93-AC7E-8516B169F1F3}"/>
-    <hyperlink ref="C5" r:id="rId9" xr:uid="{3D6E6279-A1EA-43D0-8F4B-7C87205E53DF}"/>
-    <hyperlink ref="C7" r:id="rId10" xr:uid="{2F13293B-2127-4F9F-AD29-6AC0A6164C27}"/>
-    <hyperlink ref="C9" r:id="rId11" xr:uid="{A592E3CC-17A1-414D-9E3E-D204CA51E7F7}"/>
-    <hyperlink ref="C11" r:id="rId12" xr:uid="{B2E0592E-5EF3-49CE-A0E3-B3C0ED1D452E}"/>
-    <hyperlink ref="C13" r:id="rId13" xr:uid="{F5D0115D-E85D-4CFA-89EC-11A8842E15E0}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C14" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C5" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E2" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E18" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E24" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E21" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E6" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E12" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E22" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E19" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E5" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E13" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId36"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>